<commit_message>
Advance Feature file task updates
</commit_message>
<xml_diff>
--- a/resources/resources.xlsx
+++ b/resources/resources.xlsx
@@ -127,9 +127,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>More than 30hours a week</t>
-  </si>
-  <si>
     <t>More than $1000 per month</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>SearchSkills</t>
+  </si>
+  <si>
+    <t>Less than 30hours a week</t>
   </si>
 </sst>
 </file>
@@ -690,10 +690,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" t="s">
         <v>25</v>
@@ -755,7 +755,7 @@
         <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
         <v>26</v>
@@ -772,10 +772,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>19</v>
@@ -784,10 +784,15 @@
         <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -815,22 +820,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -838,53 +843,53 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>45</v>
-      </c>
       <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
         <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>50</v>
-      </c>
-      <c r="F4" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>